<commit_message>
updated time log and project profile
</commit_message>
<xml_diff>
--- a/files/timelog.xlsx
+++ b/files/timelog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dexter Miller\Desktop\Senior-Project\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dexter\Desktop\Senior-Project\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A6D224D-7DD4-4BE3-9F8E-1754A11E094C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA3F7ED-494C-404F-A7CE-D47D3ED99BCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20193" yWindow="813" windowWidth="7500" windowHeight="6627" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7935" yWindow="3120" windowWidth="18210" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Time Recording Log</t>
   </si>
@@ -55,6 +55,27 @@
   </si>
   <si>
     <t>Iteration</t>
+  </si>
+  <si>
+    <t>logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added logo </t>
+  </si>
+  <si>
+    <t>updated logo sizes</t>
+  </si>
+  <si>
+    <t>about me page</t>
+  </si>
+  <si>
+    <t>Fixed experience text</t>
+  </si>
+  <si>
+    <t>Built connect 4 board</t>
+  </si>
+  <si>
+    <t>Total Time:</t>
   </si>
 </sst>
 </file>
@@ -101,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -113,6 +134,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -398,40 +431,45 @@
   <dimension ref="A1:H95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.41015625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="7" max="7" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20" x14ac:dyDescent="0.6">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1">
+        <f>SUM(D4:D44)</f>
+        <v>4.7500000000000018</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="2"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -455,15 +493,18 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="20" x14ac:dyDescent="0.6">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>43865</v>
+      </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1" t="str">
-        <f>IF(OR(ISBLANK(B4),ISBLANK(C4)),"",(C4-B4)*24*60-#REF!)</f>
-        <v/>
-      </c>
-      <c r="E4" s="1"/>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="3" t="str">
@@ -471,15 +512,18 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20" x14ac:dyDescent="0.6">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>43866</v>
+      </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="str">
-        <f>IF(OR(ISBLANK(B5),ISBLANK(C5)),"",(C5-B5)*24*60-#REF!)</f>
-        <v/>
-      </c>
-      <c r="E5" s="1"/>
+      <c r="D5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="3" t="str">
@@ -487,15 +531,18 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20" x14ac:dyDescent="0.6">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>43867</v>
+      </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1" t="str">
-        <f>IF(OR(ISBLANK(B6),ISBLANK(C6)),"",(C6-B6)*24*60-#REF!)</f>
-        <v/>
-      </c>
-      <c r="E6" s="1"/>
+      <c r="D6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="3" t="str">
@@ -503,15 +550,18 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="20" x14ac:dyDescent="0.6">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>43871</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1" t="str">
-        <f>IF(OR(ISBLANK(B7),ISBLANK(C7)),"",(C7-B7)*24*60-#REF!)</f>
-        <v/>
-      </c>
-      <c r="E7" s="1"/>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="3" t="str">
@@ -519,15 +569,23 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20" x14ac:dyDescent="0.6">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="str">
-        <f>IF(OR(ISBLANK(B8),ISBLANK(C8)),"",(C8-B8)*24*60-#REF!)</f>
-        <v/>
-      </c>
-      <c r="E8" s="1"/>
+    <row r="8" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>43872</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D8" s="1">
+        <f>IF(OR(ISBLANK(B8),ISBLANK(C8)),"",(C8-B8)*24)</f>
+        <v>1.0000000000000018</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="3" t="str">
@@ -535,15 +593,18 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="20" x14ac:dyDescent="0.6">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>43873</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1" t="str">
-        <f>IF(OR(ISBLANK(B9),ISBLANK(C9)),"",(C9-B9)*24*60-#REF!)</f>
-        <v/>
-      </c>
-      <c r="E9" s="1"/>
+      <c r="D9" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="3" t="str">
@@ -551,12 +612,12 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="20" x14ac:dyDescent="0.6">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+    <row r="10" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1" t="str">
-        <f>IF(OR(ISBLANK(B10),ISBLANK(C10)),"",(C10-B10)*24*60-#REF!)</f>
+      <c r="D10" s="6" t="str">
+        <f t="shared" ref="D9:D31" si="1">IF(OR(ISBLANK(B10),ISBLANK(C10)),"",(C10-B10)*24)</f>
         <v/>
       </c>
       <c r="E10" s="1"/>
@@ -567,12 +628,12 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1" t="str">
-        <f>IF(OR(ISBLANK(B11),ISBLANK(C11)),"",(C11-B11)*24*60-#REF!)</f>
+      <c r="D11" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E11" s="1"/>
@@ -583,12 +644,12 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1" t="str">
-        <f>IF(OR(ISBLANK(B12),ISBLANK(C12)),"",(C12-B12)*24*60-#REF!)</f>
+      <c r="D12" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E12" s="1"/>
@@ -599,12 +660,12 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1" t="str">
-        <f>IF(OR(ISBLANK(B13),ISBLANK(C13)),"",(C13-B13)*24*60-#REF!)</f>
+      <c r="D13" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E13" s="1"/>
@@ -615,12 +676,12 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1" t="str">
-        <f>IF(OR(ISBLANK(B14),ISBLANK(C14)),"",(C14-B14)*24*60-#REF!)</f>
+      <c r="D14" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E14" s="1"/>
@@ -631,12 +692,12 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1" t="str">
-        <f>IF(OR(ISBLANK(B15),ISBLANK(C15)),"",(C15-B15)*24*60-#REF!)</f>
+      <c r="D15" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E15" s="1"/>
@@ -647,12 +708,12 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1" t="str">
-        <f>IF(OR(ISBLANK(B16),ISBLANK(C16)),"",(C16-B16)*24*60-#REF!)</f>
+      <c r="D16" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E16" s="1"/>
@@ -663,12 +724,12 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1" t="str">
-        <f>IF(OR(ISBLANK(B17),ISBLANK(C17)),"",(C17-B17)*24*60-#REF!)</f>
+      <c r="D17" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E17" s="1"/>
@@ -679,12 +740,12 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1" t="str">
-        <f>IF(OR(ISBLANK(B18),ISBLANK(C18)),"",(C18-B18)*24*60-#REF!)</f>
+      <c r="D18" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E18" s="1"/>
@@ -695,12 +756,12 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1" t="str">
-        <f>IF(OR(ISBLANK(B19),ISBLANK(C19)),"",(C19-B19)*24*60-#REF!)</f>
+      <c r="D19" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E19" s="1"/>
@@ -711,12 +772,12 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1" t="str">
-        <f>IF(OR(ISBLANK(B20),ISBLANK(C20)),"",(C20-B20)*24*60-#REF!)</f>
+      <c r="D20" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E20" s="1"/>
@@ -727,12 +788,12 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1" t="str">
-        <f>IF(OR(ISBLANK(B21),ISBLANK(C21)),"",(C21-B21)*24*60-#REF!)</f>
+      <c r="D21" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E21" s="1"/>
@@ -743,12 +804,12 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1" t="str">
-        <f>IF(OR(ISBLANK(B22),ISBLANK(C22)),"",(C22-B22)*24*60-#REF!)</f>
+      <c r="D22" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E22" s="1"/>
@@ -759,12 +820,12 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1" t="str">
-        <f>IF(OR(ISBLANK(B23),ISBLANK(C23)),"",(C23-B23)*24*60-#REF!)</f>
+      <c r="D23" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E23" s="1"/>
@@ -775,12 +836,12 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1" t="str">
-        <f>IF(OR(ISBLANK(B24),ISBLANK(C24)),"",(C24-B24)*24*60-#REF!)</f>
+      <c r="D24" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E24" s="1"/>
@@ -791,12 +852,12 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1" t="str">
-        <f>IF(OR(ISBLANK(B25),ISBLANK(C25)),"",(C25-B25)*24*60-#REF!)</f>
+      <c r="D25" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E25" s="1"/>
@@ -807,12 +868,12 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1" t="str">
-        <f>IF(OR(ISBLANK(B26),ISBLANK(C26)),"",(C26-B26)*24*60-#REF!)</f>
+      <c r="D26" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E26" s="1"/>
@@ -823,12 +884,12 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1" t="str">
-        <f>IF(OR(ISBLANK(B27),ISBLANK(C27)),"",(C27-B27)*24*60-#REF!)</f>
+      <c r="D27" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E27" s="1"/>
@@ -839,12 +900,12 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1" t="str">
-        <f>IF(OR(ISBLANK(B28),ISBLANK(C28)),"",(C28-B28)*24*60-#REF!)</f>
+      <c r="D28" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E28" s="1"/>
@@ -855,12 +916,12 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="1" t="str">
-        <f>IF(OR(ISBLANK(B29),ISBLANK(C29)),"",(C29-B29)*24*60-#REF!)</f>
+      <c r="D29" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E29" s="1"/>
@@ -871,12 +932,12 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1" t="str">
-        <f>IF(OR(ISBLANK(B30),ISBLANK(C30)),"",(C30-B30)*24*60-#REF!)</f>
+      <c r="D30" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E30" s="1"/>
@@ -887,12 +948,12 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="1" t="str">
-        <f>IF(OR(ISBLANK(B31),ISBLANK(C31)),"",(C31-B31)*24*60-#REF!)</f>
+      <c r="D31" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E31" s="1"/>
@@ -903,7 +964,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -919,7 +980,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -935,7 +996,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -951,7 +1012,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -967,7 +1028,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="36" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -983,7 +1044,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="37" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -999,7 +1060,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="38" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1015,7 +1076,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="39" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1031,7 +1092,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="40" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1047,7 +1108,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="41" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1063,7 +1124,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="42" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1079,7 +1140,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1095,7 +1156,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1111,7 +1172,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="45" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1127,7 +1188,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="46" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1143,7 +1204,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1159,7 +1220,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="48" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1175,7 +1236,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="49" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1191,7 +1252,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="50" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1207,7 +1268,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="51" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1223,7 +1284,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="52" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1239,7 +1300,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="53" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1255,7 +1316,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="54" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1271,7 +1332,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="55" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1287,7 +1348,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="56" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1303,7 +1364,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="57" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1319,7 +1380,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="58" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1335,7 +1396,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="59" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1351,7 +1412,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="60" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1367,7 +1428,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="61" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1383,7 +1444,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="62" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1399,7 +1460,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="63" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1415,7 +1476,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="64" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1431,7 +1492,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="65" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1447,7 +1508,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="66" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1463,7 +1524,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="67" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1479,7 +1540,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+    <row r="68" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1491,11 +1552,11 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="3" t="str">
-        <f>IF(D68&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" ref="H68:H92" si="2">IF(D68&lt;0,"&lt;-- Invalid stop time","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1507,11 +1568,11 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="3" t="str">
-        <f>IF(D69&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1523,11 +1584,11 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="3" t="str">
-        <f>IF(D70&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1539,11 +1600,11 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="3" t="str">
-        <f>IF(D71&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1555,11 +1616,11 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="3" t="str">
-        <f>IF(D72&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1571,11 +1632,11 @@
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="3" t="str">
-        <f>IF(D73&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1587,11 +1648,11 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="3" t="str">
-        <f>IF(D74&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1603,11 +1664,11 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="3" t="str">
-        <f>IF(D75&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1619,11 +1680,11 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="3" t="str">
-        <f>IF(D76&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1635,11 +1696,11 @@
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="3" t="str">
-        <f>IF(D77&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1651,11 +1712,11 @@
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="3" t="str">
-        <f>IF(D78&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1667,11 +1728,11 @@
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="3" t="str">
-        <f>IF(D79&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1683,11 +1744,11 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="3" t="str">
-        <f>IF(D80&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1699,11 +1760,11 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="3" t="str">
-        <f>IF(D81&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1715,11 +1776,11 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="3" t="str">
-        <f>IF(D82&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1731,11 +1792,11 @@
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="3" t="str">
-        <f>IF(D83&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1747,11 +1808,11 @@
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="3" t="str">
-        <f>IF(D84&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1763,11 +1824,11 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="3" t="str">
-        <f>IF(D85&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1779,11 +1840,11 @@
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="3" t="str">
-        <f>IF(D86&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1795,11 +1856,11 @@
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="3" t="str">
-        <f>IF(D87&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1811,11 +1872,11 @@
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="3" t="str">
-        <f>IF(D88&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1827,11 +1888,11 @@
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="3" t="str">
-        <f>IF(D89&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1843,11 +1904,11 @@
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="3" t="str">
-        <f>IF(D90&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1859,11 +1920,11 @@
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="3" t="str">
-        <f>IF(D91&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="20" x14ac:dyDescent="0.6">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1875,11 +1936,11 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="3" t="str">
-        <f>IF(D92&lt;0,"&lt;-- Invalid stop time","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.5">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -1889,7 +1950,7 @@
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -1899,7 +1960,7 @@
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>

</xml_diff>

<commit_message>
started connect 4 js
</commit_message>
<xml_diff>
--- a/files/timelog.xlsx
+++ b/files/timelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dexter Miller\Desktop\Senior-Project\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC8F548-4375-4E29-B99B-AB300384E72C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119C4012-AC1B-41A1-81BA-F90FBBF616B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Time Recording Log</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Added a products page</t>
+  </si>
+  <si>
+    <t>Task</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
   <dimension ref="A1:H95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G17" sqref="G17:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -626,7 +629,9 @@
       <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="G3" s="13" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
column full isn't working
</commit_message>
<xml_diff>
--- a/files/timelog.xlsx
+++ b/files/timelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dexter Miller\Desktop\Senior-Project\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFF04E2-0AB5-48EA-BBED-C3F64D055E08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA5F5DE-2262-4700-8134-905804E6B1E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>Time Recording Log</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>1d</t>
+  </si>
+  <si>
+    <t>Worked on game logic</t>
   </si>
 </sst>
 </file>
@@ -591,7 +594,7 @@
   <dimension ref="A1:H95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -624,7 +627,7 @@
       </c>
       <c r="D2" s="1">
         <f>SUM(D4:D44)</f>
-        <v>11.166666666666668</v>
+        <v>12.833333333333334</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>45</v>
@@ -930,26 +933,40 @@
       <c r="F15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="G15" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="H15" s="12">
+        <f>G15-D15</f>
+        <v>2.2500000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="20" x14ac:dyDescent="0.6">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="4" t="str">
+      <c r="A16" s="5">
+        <v>43905</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.59375</v>
+      </c>
+      <c r="D16" s="4">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>1.6666666666666661</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="H16" s="12">
+        <f>H15-D16</f>
+        <v>0.58333333333333437</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="20" x14ac:dyDescent="0.6">

</xml_diff>